<commit_message>
BUGFIX01: Excel template had a line incorrectly saying that cables were exceeding containment at all times. BUGFIX02: Confirm that if there's no self.filename the software still offers the options for saveas on confirm exit.
</commit_message>
<xml_diff>
--- a/TemplateContCalc.xlsx
+++ b/TemplateContCalc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao\Documents\contcalc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.jesus\Documents\contcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8070EEF-91E7-4277-A64D-D46B25C3F50D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4428FCA1-0A06-4B38-86C8-9B050AC99637}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="688" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="145" r:id="rId1"/>
@@ -383,68 +383,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -508,6 +446,68 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,16 +632,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>100964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>220601</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>77936</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>838199</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6935</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -664,8 +664,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76200" y="129540"/>
-          <a:ext cx="915926" cy="329396"/>
+          <a:off x="171449" y="100964"/>
+          <a:ext cx="1857375" cy="667971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D2238D-166D-412B-9B4D-3D42AEA0F376}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,14 +1183,14 @@
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="38"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="62"/>
       <c r="L9" s="7"/>
       <c r="O9" s="31"/>
       <c r="P9" s="31"/>
@@ -1229,10 +1229,10 @@
         <v>21</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="7"/>
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
@@ -1271,10 +1271,10 @@
         <v>22</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="65"/>
       <c r="L13" s="7"/>
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
@@ -1302,17 +1302,17 @@
       <c r="S14" s="31"/>
     </row>
     <row r="15" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
       <c r="L15" s="31"/>
       <c r="O15" s="31"/>
       <c r="P15" s="31"/>
@@ -1321,17 +1321,17 @@
       <c r="S15" s="31"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
       <c r="L16" s="31"/>
       <c r="O16" s="31"/>
       <c r="P16" s="31"/>
@@ -1340,17 +1340,17 @@
       <c r="S16" s="31"/>
     </row>
     <row r="17" spans="1:19" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="O17" s="31"/>
@@ -1360,17 +1360,17 @@
       <c r="S17" s="31"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="54"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="54"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="36"/>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="O18" s="31"/>
@@ -1380,17 +1380,17 @@
       <c r="S18" s="31"/>
     </row>
     <row r="19" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="54"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="36"/>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="O19" s="31"/>
@@ -1400,17 +1400,17 @@
       <c r="S19" s="31"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="62"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="44"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="54"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="36"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="O20" s="31"/>
@@ -1420,17 +1420,17 @@
       <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="54"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="36"/>
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="O21" s="31"/>
@@ -1440,17 +1440,17 @@
       <c r="S21" s="31"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="54"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="36"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="O22" s="31"/>
@@ -1460,17 +1460,17 @@
       <c r="S22" s="31"/>
     </row>
     <row r="23" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="O23" s="31"/>
@@ -1480,17 +1480,17 @@
       <c r="S23" s="31"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="65"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="47"/>
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
       <c r="O24" s="31"/>
@@ -1500,17 +1500,17 @@
       <c r="S24" s="31"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="70"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="52"/>
       <c r="L25" s="17"/>
       <c r="M25" s="17"/>
       <c r="O25" s="31"/>
@@ -1520,17 +1520,17 @@
       <c r="S25" s="31"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="70"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="52"/>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
       <c r="O26" s="31"/>
@@ -1540,17 +1540,17 @@
       <c r="S26" s="31"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="70"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="52"/>
       <c r="L27" s="17"/>
       <c r="M27" s="17"/>
       <c r="O27" s="31"/>
@@ -1560,17 +1560,17 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="70"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="52"/>
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
@@ -1581,17 +1581,17 @@
       <c r="S28" s="31"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="70"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="52"/>
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
@@ -1602,17 +1602,17 @@
       <c r="S29" s="31"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="70"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="52"/>
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
@@ -1623,17 +1623,17 @@
       <c r="S30" s="31"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="70"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="52"/>
       <c r="L31" s="17"/>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
@@ -1644,17 +1644,17 @@
       <c r="S31" s="31"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="70"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="52"/>
       <c r="L32" s="17"/>
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
@@ -1665,17 +1665,17 @@
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="70"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="52"/>
       <c r="L33" s="17"/>
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
@@ -1686,17 +1686,17 @@
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="70"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="52"/>
       <c r="L34" s="17"/>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
@@ -1707,17 +1707,17 @@
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="68"/>
-      <c r="J35" s="68"/>
-      <c r="K35" s="70"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="52"/>
       <c r="L35" s="17"/>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -1728,17 +1728,17 @@
       <c r="S35" s="31"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="70"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="52"/>
       <c r="L36" s="17"/>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -1749,17 +1749,17 @@
       <c r="S36" s="31"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
-      <c r="B37" s="67"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="70"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="52"/>
       <c r="L37" s="17"/>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
@@ -1770,17 +1770,17 @@
       <c r="S37" s="31"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
-      <c r="B38" s="67"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="70"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="52"/>
       <c r="L38" s="17"/>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
@@ -1791,17 +1791,17 @@
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="70"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="52"/>
       <c r="L39" s="17"/>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
@@ -1812,17 +1812,17 @@
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="68"/>
-      <c r="K40" s="70"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="52"/>
       <c r="L40" s="17"/>
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
@@ -1833,17 +1833,17 @@
       <c r="S40" s="31"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="70"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="52"/>
       <c r="L41" s="17"/>
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
@@ -1854,17 +1854,17 @@
       <c r="S41" s="31"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
-      <c r="B42" s="67"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="70"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
+      <c r="K42" s="52"/>
       <c r="L42" s="17"/>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
@@ -1875,17 +1875,17 @@
       <c r="S42" s="31"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
-      <c r="B43" s="67"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="69"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="70"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="52"/>
       <c r="L43" s="17"/>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
@@ -1896,17 +1896,17 @@
       <c r="S43" s="31"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="70"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="52"/>
       <c r="L44" s="17"/>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
@@ -1917,17 +1917,17 @@
       <c r="S44" s="31"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
-      <c r="B45" s="67"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="68"/>
-      <c r="J45" s="68"/>
-      <c r="K45" s="70"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="52"/>
       <c r="L45" s="17"/>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
@@ -1938,17 +1938,17 @@
       <c r="S45" s="31"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="54"/>
-      <c r="K46" s="54"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
       <c r="L46" s="17"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
@@ -1959,17 +1959,17 @@
       <c r="S46" s="31"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
-      <c r="B47" s="54"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="73"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="55"/>
       <c r="L47" s="17"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -1980,17 +1980,17 @@
       <c r="S47" s="31"/>
     </row>
     <row r="48" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="54"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="54"/>
-      <c r="G48" s="54"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="54"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
       <c r="L48" s="17"/>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
@@ -2001,17 +2001,17 @@
       <c r="S48" s="31"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="71"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="72"/>
-      <c r="K49" s="73"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="55"/>
       <c r="L49" s="17"/>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
@@ -2022,17 +2022,17 @@
       <c r="S49" s="31"/>
     </row>
     <row r="50" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54"/>
-      <c r="B50" s="54"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="54"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
       <c r="I50" s="17"/>
-      <c r="J50" s="54"/>
-      <c r="K50" s="54"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
       <c r="L50" s="17"/>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
@@ -2043,20 +2043,20 @@
       <c r="S50" s="31"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="54"/>
-      <c r="B51" s="54"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="74"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="73"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="55"/>
       <c r="L51" s="17"/>
       <c r="M51" s="17"/>
-      <c r="N51" s="77"/>
+      <c r="N51" s="59"/>
       <c r="O51" s="31"/>
       <c r="P51" s="31"/>
       <c r="Q51" s="31"/>
@@ -2074,7 +2074,7 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
       <c r="J52" s="17"/>
-      <c r="K52" s="75"/>
+      <c r="K52" s="57"/>
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
@@ -2086,8 +2086,8 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
-      <c r="B53" s="76"/>
-      <c r="C53" s="76"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
@@ -2440,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,8 +2637,8 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="74"/>
       <c r="K9" s="5"/>
       <c r="L9" s="7"/>
       <c r="O9" s="31"/>
@@ -2671,24 +2671,24 @@
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="45"/>
+      <c r="D11" s="76"/>
       <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="G11" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="44" t="s">
+      <c r="H11" s="77"/>
+      <c r="I11" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="46"/>
+      <c r="J11" s="77"/>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2702,14 +2702,14 @@
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="35"/>
       <c r="F12" s="35"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="48"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="70"/>
       <c r="K12" s="24"/>
       <c r="L12" s="7"/>
       <c r="O12" s="31"/>
@@ -2721,14 +2721,14 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="34"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="48"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="70"/>
       <c r="K13" s="24"/>
       <c r="L13" s="7"/>
       <c r="O13" s="31"/>
@@ -2740,14 +2740,14 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="34"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="70"/>
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="48"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="70"/>
       <c r="K14" s="24"/>
       <c r="L14" s="7"/>
       <c r="O14" s="31"/>
@@ -2759,14 +2759,14 @@
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="34"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="70"/>
       <c r="E15" s="35"/>
       <c r="F15" s="35"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="48"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="70"/>
       <c r="K15" s="24"/>
       <c r="L15" s="7"/>
       <c r="O15" s="31"/>
@@ -2778,14 +2778,14 @@
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="34"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="70"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="48"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="70"/>
       <c r="K16" s="24"/>
       <c r="L16" s="7"/>
       <c r="O16" s="31"/>
@@ -2797,14 +2797,14 @@
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="34"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="70"/>
       <c r="E17" s="35"/>
       <c r="F17" s="35"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="70"/>
       <c r="K17" s="24"/>
       <c r="L17" s="7"/>
       <c r="O17" s="31"/>
@@ -2816,14 +2816,14 @@
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="34"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="70"/>
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="48"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="70"/>
       <c r="K18" s="24"/>
       <c r="L18" s="7"/>
       <c r="O18" s="31"/>
@@ -2835,14 +2835,14 @@
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="48"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="70"/>
       <c r="K19" s="24"/>
       <c r="L19" s="7"/>
       <c r="O19" s="31"/>
@@ -2854,14 +2854,14 @@
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="34"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="70"/>
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="48"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="70"/>
       <c r="K20" s="24"/>
       <c r="L20" s="7"/>
       <c r="O20" s="31"/>
@@ -2873,14 +2873,14 @@
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="34"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="48"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="70"/>
       <c r="K21" s="24"/>
       <c r="L21" s="7"/>
       <c r="O21" s="31"/>
@@ -2892,14 +2892,14 @@
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="34"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="70"/>
       <c r="E22" s="35"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="48"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="70"/>
       <c r="K22" s="24"/>
       <c r="L22" s="7"/>
       <c r="O22" s="31"/>
@@ -2911,14 +2911,14 @@
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="34"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="70"/>
       <c r="E23" s="35"/>
       <c r="F23" s="35"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="48"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="70"/>
       <c r="K23" s="24"/>
       <c r="L23" s="7"/>
       <c r="O23" s="31"/>
@@ -2930,14 +2930,14 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="34"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="70"/>
       <c r="E24" s="35"/>
       <c r="F24" s="35"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="48"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="70"/>
       <c r="K24" s="24"/>
       <c r="L24" s="7"/>
       <c r="O24" s="31"/>
@@ -2949,14 +2949,14 @@
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="34"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="70"/>
       <c r="E25" s="35"/>
       <c r="F25" s="35"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="48"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="70"/>
       <c r="K25" s="24"/>
       <c r="L25" s="7"/>
       <c r="O25" s="31"/>
@@ -2968,14 +2968,14 @@
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="34"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="70"/>
       <c r="E26" s="35"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="70"/>
       <c r="K26" s="24"/>
       <c r="L26" s="7"/>
       <c r="O26" s="31"/>
@@ -2987,14 +2987,14 @@
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="34"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="70"/>
       <c r="E27" s="35"/>
       <c r="F27" s="35"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="48"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="70"/>
       <c r="K27" s="24"/>
       <c r="L27" s="7"/>
       <c r="O27" s="31"/>
@@ -3006,14 +3006,14 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="34"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="49"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="69"/>
       <c r="E28" s="35"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="48"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="70"/>
       <c r="K28" s="24"/>
       <c r="L28" s="7"/>
       <c r="O28" s="31"/>
@@ -3025,14 +3025,14 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="34"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="49"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="69"/>
       <c r="E29" s="35"/>
       <c r="F29" s="35"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="48"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="70"/>
       <c r="K29" s="24"/>
       <c r="L29" s="7"/>
       <c r="O29" s="31"/>
@@ -3044,14 +3044,14 @@
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="34"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="49"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="69"/>
       <c r="E30" s="35"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="48"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="70"/>
       <c r="K30" s="24"/>
       <c r="L30" s="7"/>
       <c r="O30" s="31"/>
@@ -3063,14 +3063,14 @@
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="34"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="49"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="69"/>
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="48"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="70"/>
       <c r="K31" s="24"/>
       <c r="L31" s="7"/>
       <c r="O31" s="31"/>
@@ -3082,14 +3082,14 @@
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="34"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="49"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="69"/>
       <c r="E32" s="35"/>
       <c r="F32" s="35"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="48"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="70"/>
       <c r="K32" s="24"/>
       <c r="L32" s="7"/>
       <c r="O32" s="31"/>
@@ -3128,8 +3128,8 @@
       <c r="H34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="52"/>
-      <c r="J34" s="53"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="72"/>
       <c r="K34" s="22" t="s">
         <v>10</v>
       </c>
@@ -3170,8 +3170,8 @@
       <c r="H36" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="52"/>
-      <c r="J36" s="53"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="72"/>
       <c r="K36" s="22" t="s">
         <v>10</v>
       </c>
@@ -3213,8 +3213,8 @@
         <f>CONCATENATE("Standard containment size required (",D7,"):  ")</f>
         <v xml:space="preserve">Standard containment size required ():  </v>
       </c>
-      <c r="I38" s="50"/>
-      <c r="J38" s="51"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="67"/>
       <c r="K38" s="23" t="s">
         <v>10</v>
       </c>
@@ -3237,10 +3237,7 @@
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
-      <c r="K39" s="26" t="str">
-        <f>IF(I36&gt;900, "Too many cables to fit on a standard containment size. Consider splitting cables.", "")</f>
-        <v/>
-      </c>
+      <c r="K39" s="26"/>
       <c r="L39" s="9"/>
       <c r="O39" s="31"/>
       <c r="P39" s="31"/>
@@ -3479,6 +3476,64 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="70">
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="G30:H30"/>
@@ -3491,64 +3546,6 @@
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="I36:J36"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="N21 K16:K18">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">

</xml_diff>

<commit_message>
BUGFIX03: Update image placement
</commit_message>
<xml_diff>
--- a/TemplateContCalc.xlsx
+++ b/TemplateContCalc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.jesus\Documents\contcalc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao\Documents\contcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4428FCA1-0A06-4B38-86C8-9B050AC99637}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D725A9B6-58C8-4E26-A2EB-870906C63270}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,27 +470,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -507,6 +486,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,55 +626,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>100964</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>838199</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>6935</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Arup26mm.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78227908-71E3-4F64-8366-38BF2A32E8E9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="171449" y="100964"/>
-          <a:ext cx="1857375" cy="667971"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2432,7 +2383,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2637,8 +2587,8 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="74"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="67"/>
       <c r="K9" s="5"/>
       <c r="L9" s="7"/>
       <c r="O9" s="31"/>
@@ -2671,24 +2621,24 @@
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="76"/>
+      <c r="D11" s="69"/>
       <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="77"/>
-      <c r="I11" s="75" t="s">
+      <c r="H11" s="70"/>
+      <c r="I11" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="77"/>
+      <c r="J11" s="70"/>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2702,14 +2652,14 @@
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="35"/>
       <c r="F12" s="35"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="72"/>
       <c r="K12" s="24"/>
       <c r="L12" s="7"/>
       <c r="O12" s="31"/>
@@ -2721,14 +2671,14 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="34"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="70"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="70"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="72"/>
       <c r="K13" s="24"/>
       <c r="L13" s="7"/>
       <c r="O13" s="31"/>
@@ -2740,14 +2690,14 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="34"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="70"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="72"/>
       <c r="K14" s="24"/>
       <c r="L14" s="7"/>
       <c r="O14" s="31"/>
@@ -2759,14 +2709,14 @@
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="34"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="70"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="35"/>
       <c r="F15" s="35"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="72"/>
       <c r="K15" s="24"/>
       <c r="L15" s="7"/>
       <c r="O15" s="31"/>
@@ -2778,14 +2728,14 @@
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="34"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="70"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="70"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="72"/>
       <c r="K16" s="24"/>
       <c r="L16" s="7"/>
       <c r="O16" s="31"/>
@@ -2797,14 +2747,14 @@
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="34"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="70"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="35"/>
       <c r="F17" s="35"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="70"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="72"/>
       <c r="K17" s="24"/>
       <c r="L17" s="7"/>
       <c r="O17" s="31"/>
@@ -2816,14 +2766,14 @@
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="34"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="70"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="70"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="72"/>
       <c r="K18" s="24"/>
       <c r="L18" s="7"/>
       <c r="O18" s="31"/>
@@ -2835,14 +2785,14 @@
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="70"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="70"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="72"/>
       <c r="K19" s="24"/>
       <c r="L19" s="7"/>
       <c r="O19" s="31"/>
@@ -2854,14 +2804,14 @@
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="34"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="70"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="72"/>
       <c r="K20" s="24"/>
       <c r="L20" s="7"/>
       <c r="O20" s="31"/>
@@ -2873,14 +2823,14 @@
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="34"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="70"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="72"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="70"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="72"/>
       <c r="K21" s="24"/>
       <c r="L21" s="7"/>
       <c r="O21" s="31"/>
@@ -2892,14 +2842,14 @@
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="34"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="70"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="35"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="70"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="72"/>
       <c r="K22" s="24"/>
       <c r="L22" s="7"/>
       <c r="O22" s="31"/>
@@ -2911,14 +2861,14 @@
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="34"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="70"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="72"/>
       <c r="E23" s="35"/>
       <c r="F23" s="35"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="70"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="72"/>
       <c r="K23" s="24"/>
       <c r="L23" s="7"/>
       <c r="O23" s="31"/>
@@ -2930,14 +2880,14 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="34"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="70"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="35"/>
       <c r="F24" s="35"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="70"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="72"/>
       <c r="K24" s="24"/>
       <c r="L24" s="7"/>
       <c r="O24" s="31"/>
@@ -2949,14 +2899,14 @@
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="34"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="70"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="35"/>
       <c r="F25" s="35"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="70"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="72"/>
       <c r="K25" s="24"/>
       <c r="L25" s="7"/>
       <c r="O25" s="31"/>
@@ -2968,14 +2918,14 @@
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="34"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="70"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="35"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="70"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="72"/>
       <c r="K26" s="24"/>
       <c r="L26" s="7"/>
       <c r="O26" s="31"/>
@@ -2987,14 +2937,14 @@
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="34"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="70"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="35"/>
       <c r="F27" s="35"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="72"/>
       <c r="K27" s="24"/>
       <c r="L27" s="7"/>
       <c r="O27" s="31"/>
@@ -3006,14 +2956,14 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="34"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="69"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="35"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="72"/>
       <c r="K28" s="24"/>
       <c r="L28" s="7"/>
       <c r="O28" s="31"/>
@@ -3025,14 +2975,14 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="34"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="69"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="35"/>
       <c r="F29" s="35"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="72"/>
       <c r="K29" s="24"/>
       <c r="L29" s="7"/>
       <c r="O29" s="31"/>
@@ -3044,14 +2994,14 @@
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="34"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="73"/>
       <c r="E30" s="35"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="70"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="72"/>
       <c r="K30" s="24"/>
       <c r="L30" s="7"/>
       <c r="O30" s="31"/>
@@ -3063,14 +3013,14 @@
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="34"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="69"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="73"/>
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="70"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="72"/>
       <c r="K31" s="24"/>
       <c r="L31" s="7"/>
       <c r="O31" s="31"/>
@@ -3082,14 +3032,14 @@
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="34"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="69"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="35"/>
       <c r="F32" s="35"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="70"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="72"/>
       <c r="K32" s="24"/>
       <c r="L32" s="7"/>
       <c r="O32" s="31"/>
@@ -3128,8 +3078,8 @@
       <c r="H34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="71"/>
-      <c r="J34" s="72"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="77"/>
       <c r="K34" s="22" t="s">
         <v>10</v>
       </c>
@@ -3170,8 +3120,8 @@
       <c r="H36" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="71"/>
-      <c r="J36" s="72"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="77"/>
       <c r="K36" s="22" t="s">
         <v>10</v>
       </c>
@@ -3213,8 +3163,8 @@
         <f>CONCATENATE("Standard containment size required (",D7,"):  ")</f>
         <v xml:space="preserve">Standard containment size required ():  </v>
       </c>
-      <c r="I38" s="66"/>
-      <c r="J38" s="67"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="75"/>
       <c r="K38" s="23" t="s">
         <v>10</v>
       </c>
@@ -3476,61 +3426,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="70">
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:J29"/>
@@ -3546,6 +3441,61 @@
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="I36:J36"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <conditionalFormatting sqref="N21 K16:K18">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">

</xml_diff>